<commit_message>
- IND_97 Add error column - Add BR details
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Action</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>LIB_EWS</t>
+  </si>
+  <si>
+    <t>getExpressionQuery</t>
+  </si>
+  <si>
+    <t>String,String</t>
   </si>
 </sst>
 </file>
@@ -762,10 +768,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -855,6 +861,20 @@
         <v>15</v>
       </c>
       <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -900,6 +920,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1013,22 +1048,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1042,27 +1085,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update to framework 7.1
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Action</t>
   </si>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -863,6 +863,9 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
@@ -920,21 +923,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1048,10 +1036,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1072,17 +1083,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix new output table for Visual modeling and matrix
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
   <si>
     <t>Action</t>
   </si>
@@ -197,11 +197,14 @@
   <si>
     <t>getMaxColor</t>
   </si>
+  <si>
+    <t>UpdatePredictiveModel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -795,10 +798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1056,6 +1059,23 @@
         <v>15</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1103,6 +1123,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1216,22 +1251,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1245,27 +1288,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
check analysis unit status
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="33">
   <si>
     <t>Action</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>UpdatePredictiveModel</t>
+  </si>
+  <si>
+    <t>checkAnalysisUnitStatus</t>
   </si>
 </sst>
 </file>
@@ -798,10 +801,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1076,6 +1079,23 @@
         <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1123,21 +1143,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1251,10 +1256,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1275,17 +1303,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- FIX output BE ( ADD Schema ) - New feature for output IT
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="36">
   <si>
     <t>Action</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>UpdateWorkpalceTable</t>
+  </si>
+  <si>
+    <t>getVMNodeColumnByName</t>
   </si>
 </sst>
 </file>
@@ -807,10 +810,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1137,6 +1140,23 @@
       </c>
       <c r="F18" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1183,6 +1203,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1296,22 +1331,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1325,27 +1368,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
FIX update VM table
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>Action</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>getVMNodeColumnByName</t>
+  </si>
+  <si>
+    <t>UpdateVMTable</t>
   </si>
 </sst>
 </file>
@@ -328,7 +331,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -371,7 +380,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -424,7 +439,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2052" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="2052" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -467,7 +488,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 4"/>
+        <xdr:cNvPr id="2" name="AutoShape 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -810,10 +837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1156,6 +1183,23 @@
         <v>15</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1203,21 +1247,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1331,10 +1360,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1355,17 +1407,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Calculate BR values for all Analysis unit output
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/03_LIB_EWS/03_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="38">
   <si>
     <t>Action</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>UpdateVMTable</t>
+  </si>
+  <si>
+    <t>getBRFieldName</t>
   </si>
 </sst>
 </file>
@@ -837,10 +840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1200,6 +1203,23 @@
         <v>15</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1247,6 +1267,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1360,22 +1395,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1389,27 +1432,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>